<commit_message>
Small correction to ferrite description.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/stepper driver/stepper driver BOM.xlsx
+++ b/Hardware/PCB/stepper driver/stepper driver BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\harp-tech\device.stepperdriver\Hardware\PCB\stepper driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0323307E-E710-4A22-B8E1-FBFA44DDAA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD92BFE8-F4BA-4B72-8991-792277FB2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="306" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="306" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stepper driver BOM" sheetId="5" r:id="rId1"/>
@@ -257,9 +257,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>400R@100MHz</t>
-  </si>
-  <si>
     <t>MI0805K400R-10</t>
   </si>
   <si>
@@ -636,6 +633,9 @@
   </si>
   <si>
     <t>stepper driver BOM v1.0</t>
+  </si>
+  <si>
+    <t>40R@100MHz</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66885FA-F4D0-4646-9AF7-F59BEA14699B}">
   <dimension ref="A2:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
   <sheetData>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1048,13 +1048,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -1068,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1088,16 +1088,16 @@
         <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
@@ -1108,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -1128,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
@@ -1148,7 +1148,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -1188,16 +1188,16 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>23</v>
@@ -1208,16 +1208,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>7</v>
@@ -1228,16 +1228,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>7</v>
@@ -1248,16 +1248,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
@@ -1268,16 +1268,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>7</v>
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>28</v>
@@ -1308,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>28</v>
@@ -1348,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>34</v>
@@ -1388,16 +1388,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>7</v>
@@ -1414,7 +1414,7 @@
         <v>41</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>42</v>
@@ -1468,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>50</v>
@@ -1494,7 +1494,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>53</v>
@@ -1508,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>54</v>
@@ -1548,7 +1548,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>61</v>
@@ -1574,10 +1574,10 @@
         <v>65</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>7</v>
@@ -1591,13 +1591,13 @@
         <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>7</v>
@@ -1608,16 +1608,16 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>7</v>
@@ -1628,16 +1628,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>23</v>
@@ -1648,16 +1648,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>7</v>
@@ -1668,16 +1668,16 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>7</v>
@@ -1688,16 +1688,16 @@
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>7</v>
@@ -1708,16 +1708,16 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>7</v>
@@ -1728,16 +1728,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="E39" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>7</v>
@@ -1748,16 +1748,16 @@
         <v>9</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>7</v>
@@ -1768,16 +1768,16 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>7</v>
@@ -1788,16 +1788,16 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>7</v>
@@ -1808,16 +1808,16 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>7</v>
@@ -1828,16 +1828,16 @@
         <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>7</v>
@@ -1848,16 +1848,16 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>7</v>
@@ -1868,16 +1868,16 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>7</v>
@@ -1888,16 +1888,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>7</v>
@@ -1908,16 +1908,16 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>7</v>
@@ -1928,16 +1928,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>7</v>
@@ -1948,16 +1948,16 @@
         <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>7</v>
@@ -1968,16 +1968,16 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="E51" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>7</v>
@@ -1988,16 +1988,16 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>23</v>
@@ -2008,16 +2008,16 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>7</v>
@@ -2028,16 +2028,16 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>7</v>
@@ -2048,16 +2048,16 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Replaced front LED resistors with the final values.
Reduced LED brightness for appropriate light to be used on vivariums.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/stepper driver/stepper driver BOM.xlsx
+++ b/Hardware/PCB/stepper driver/stepper driver BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\harp-tech\device.stepperdriver\Hardware\PCB\stepper driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B399A499-B203-44F9-8458-ECFCA9AF24DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9462370A-6893-4C59-9737-466CBD6D59DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="306" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="306" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stepper driver BOM" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="201">
   <si>
     <t>Value</t>
   </si>
@@ -332,15 +332,6 @@
     <t>OEPS020041</t>
   </si>
   <si>
-    <t>330R</t>
-  </si>
-  <si>
-    <t>RC0402FR-07330RL</t>
-  </si>
-  <si>
-    <t>OEPS020037</t>
-  </si>
-  <si>
     <t>12k</t>
   </si>
   <si>
@@ -503,12 +494,6 @@
     <t>C2-C13, C15, C17-C19, C23, C24, C27, C28, C30, C35, C36, C38, C39, C41-C45, C48, C51, C60, C63, C66-C71, C74, C77, C86, C89, C92-C95</t>
   </si>
   <si>
-    <t>CLKIN1</t>
-  </si>
-  <si>
-    <t>CLKOUT1</t>
-  </si>
-  <si>
     <t>D2, D3</t>
   </si>
   <si>
@@ -660,6 +645,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>CLKIN1, CLKOUT1</t>
+  </si>
+  <si>
+    <t>2k4</t>
+  </si>
+  <si>
+    <t>OEPS020089</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF2401X</t>
   </si>
 </sst>
 </file>
@@ -775,8 +772,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4BEB417-141B-4290-84CB-C876450A0E75}" name="stepper_driver__4" displayName="stepper_driver__4" ref="A5:F55" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A5:F55" xr:uid="{B4BEB417-141B-4290-84CB-C876450A0E75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B4BEB417-141B-4290-84CB-C876450A0E75}" name="stepper_driver__4" displayName="stepper_driver__4" ref="A5:F54" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A5:F54" xr:uid="{B4BEB417-141B-4290-84CB-C876450A0E75}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{95F413ED-D9A2-4694-9B1D-F53B9F21086B}" name="Qty" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{8CF59EE7-8ECE-444C-8BF9-400EDDA6BF57}" name="Reference(s)" dataDxfId="4"/>
@@ -1052,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66885FA-F4D0-4646-9AF7-F59BEA14699B}">
-  <dimension ref="A2:F60"/>
+  <dimension ref="A2:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1074,7 +1071,7 @@
   <sheetData>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,13 +1079,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -1102,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1122,16 +1119,16 @@
         <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
@@ -1142,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -1162,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
@@ -1182,7 +1179,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -1222,16 +1219,16 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>23</v>
@@ -1242,16 +1239,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>7</v>
@@ -1262,16 +1259,16 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>7</v>
@@ -1282,16 +1279,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
@@ -1302,16 +1299,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>7</v>
@@ -1319,10 +1316,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>28</v>
@@ -1342,16 +1339,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>150</v>
+        <v>31</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>7</v>
@@ -1359,19 +1356,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>7</v>
@@ -1379,19 +1376,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>7</v>
@@ -1402,16 +1399,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>38</v>
+        <v>181</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>7</v>
@@ -1422,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>187</v>
+        <v>40</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>7</v>
@@ -1442,16 +1439,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>7</v>
@@ -1462,16 +1459,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>7</v>
@@ -1479,19 +1476,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>7</v>
@@ -1499,19 +1496,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>7</v>
@@ -1519,19 +1516,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>168</v>
+        <v>56</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>7</v>
@@ -1539,19 +1536,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>7</v>
@@ -1559,42 +1556,42 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,16 +1599,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>65</v>
+        <v>186</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>169</v>
+        <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>7</v>
@@ -1622,336 +1619,340 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>191</v>
+        <v>117</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <f>stepper_driver__4[[#This Row],[Qty]]*20</f>
         <v>120</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>1</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>22</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>6</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>1</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>1</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>9</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>1</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>6</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="F43" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
         <v>4</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>8</v>
-      </c>
       <c r="B44" s="1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="D47" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="F47" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>7</v>
@@ -1959,10 +1960,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>105</v>
@@ -1979,19 +1980,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>7</v>
@@ -2002,10 +2003,10 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>112</v>
@@ -2014,27 +2015,27 @@
         <v>111</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2042,16 +2043,16 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>7</v>
@@ -2062,78 +2063,58 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
         <v>192</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <v>1</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>195</v>
+      <c r="D58" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>189</v>
+      </c>
+      <c r="F58" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D59" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E59" t="s">
         <v>194</v>
       </c>
       <c r="F59" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
-        <v>200</v>
-      </c>
-      <c r="D60" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" t="s">
-        <v>199</v>
-      </c>
-      <c r="F60" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>